<commit_message>
mostrar la primera pregunta
</commit_message>
<xml_diff>
--- a/src/files/BD.xlsx
+++ b/src/files/BD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janus\Documents\GitHub\ProyectoFinalPoo\src\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arang\Downloads\ProyectoFinalPoo\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D4EB21-864B-4700-8072-A111D2948920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5354A2E1-37EA-42EB-BF2F-DB631016893E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{98DE0EC7-51D9-420C-A038-21A631DBCF84}"/>
   </bookViews>
@@ -383,7 +383,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,7 +398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,18 +409,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -559,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -579,25 +567,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -615,19 +603,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -772,8 +751,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FFFA1768-5FAF-4578-8DE0-3F1BFAA92D71}" name="Table2" displayName="Table2" ref="A1:D60" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D60" xr:uid="{FFFA1768-5FAF-4578-8DE0-3F1BFAA92D71}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FFFA1768-5FAF-4578-8DE0-3F1BFAA92D71}" name="Table2" displayName="Table2" ref="A1:D49" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D49" xr:uid="{FFFA1768-5FAF-4578-8DE0-3F1BFAA92D71}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1F8EB648-9598-45BF-8175-EBD0DC0F3BA9}" name="id" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{515D636B-AF71-4214-BD19-494593935D8B}" name="Opcion" dataDxfId="2"/>
@@ -1107,15 +1086,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="60" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.75" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="3"/>
-    <col min="4" max="16384" width="9.125" style="4"/>
+    <col min="1" max="1" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" customHeight="1">
+    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1137,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60" customHeight="1">
+    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1148,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" customHeight="1">
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1159,7 +1138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" customHeight="1">
+    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1170,7 +1149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" customHeight="1">
+    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1181,7 +1160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" customHeight="1">
+    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1192,7 +1171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1">
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1203,7 +1182,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="60" customHeight="1">
+    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1214,7 +1193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="60" customHeight="1">
+    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1225,7 +1204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="60" customHeight="1">
+    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1236,7 +1215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="60" customHeight="1">
+    <row r="12" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1247,7 +1226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60" customHeight="1">
+    <row r="13" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1269,20 +1248,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B70C11-B6DB-4E42-8D48-D43A2A7EC852}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="60" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="60.75" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="5"/>
+    <col min="2" max="3" width="60.7109375" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
@@ -1296,7 +1275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60" customHeight="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -1310,7 +1289,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60" customHeight="1">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>1</v>
       </c>
@@ -1324,7 +1303,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" customHeight="1">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -1338,7 +1317,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" customHeight="1">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>1</v>
       </c>
@@ -1352,688 +1331,623 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="3" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:4" ht="60" customHeight="1">
-      <c r="A7" s="8">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D6" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60" customHeight="1">
-      <c r="A8" s="21">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
         <v>2</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D7" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" customHeight="1">
-      <c r="A9" s="21">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D8" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" customHeight="1">
-      <c r="A10" s="21">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
         <v>2</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D9" s="11">
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="3" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:4" ht="60" customHeight="1">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D12" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="60" customHeight="1">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13" s="10">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>4</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" customHeight="1">
-      <c r="A14" s="17">
-        <v>3</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="10">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="60" customHeight="1">
-      <c r="A15" s="17">
-        <v>3</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="10">
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="11">
         <v>-100</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="3" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" spans="1:4" ht="60" customHeight="1">
-      <c r="A17" s="21">
-        <v>4</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="12">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>5</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60" customHeight="1">
-      <c r="A18" s="21">
-        <v>4</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" s="11">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>5</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="60" customHeight="1">
-      <c r="A19" s="21">
-        <v>4</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="12">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>5</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="60" customHeight="1">
-      <c r="A20" s="21">
-        <v>4</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="11">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>5</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="11">
         <v>-100</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="3" customHeight="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-    </row>
-    <row r="22" spans="1:4" ht="60" customHeight="1">
-      <c r="A22" s="17">
-        <v>5</v>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
+        <v>6</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D22" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="60" customHeight="1">
-      <c r="A23" s="17">
-        <v>5</v>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <v>6</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D23" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="60" customHeight="1">
-      <c r="A24" s="17">
-        <v>5</v>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <v>6</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D24" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="60" customHeight="1">
-      <c r="A25" s="17">
-        <v>5</v>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>6</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D25" s="11">
         <v>-100</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="3" customHeight="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-    </row>
-    <row r="27" spans="1:4" ht="60" customHeight="1">
-      <c r="A27" s="21">
-        <v>6</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="12">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>7</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="60" customHeight="1">
-      <c r="A28" s="21">
-        <v>6</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="11">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>7</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="60" customHeight="1">
-      <c r="A29" s="21">
-        <v>6</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="12">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>7</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="60" customHeight="1">
-      <c r="A30" s="21">
-        <v>6</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="11">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <v>7</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="11">
         <v>-100</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="3" customHeight="1">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-    </row>
-    <row r="32" spans="1:4" ht="60" customHeight="1">
-      <c r="A32" s="17">
-        <v>7</v>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
+        <v>8</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
+        <v>8</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
+        <v>8</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>84</v>
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="D32" s="12">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <v>8</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="11">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="19">
+        <v>9</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="60" customHeight="1">
-      <c r="A33" s="17">
-        <v>7</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="11">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="19">
+        <v>9</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="60" customHeight="1">
-      <c r="A34" s="17">
-        <v>7</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="12">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="19">
+        <v>9</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="60" customHeight="1">
-      <c r="A35" s="17">
-        <v>7</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" s="11">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="19">
+        <v>9</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="11">
         <v>-100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="3" customHeight="1">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-    </row>
-    <row r="37" spans="1:4" ht="60" customHeight="1">
-      <c r="A37" s="21">
-        <v>8</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="12">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <v>10</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="60" customHeight="1">
-      <c r="A38" s="21">
-        <v>8</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="11">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="18">
+        <v>10</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="60" customHeight="1">
-      <c r="A39" s="21">
-        <v>8</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="12">
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="18">
+        <v>10</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="60" customHeight="1">
-      <c r="A40" s="21">
-        <v>8</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="11">
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="18">
+        <v>10</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="11">
         <v>-100</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="3" customHeight="1">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-    </row>
-    <row r="42" spans="1:4" ht="60" customHeight="1">
-      <c r="A42" s="22">
-        <v>9</v>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="19">
+        <v>11</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>93</v>
+        <v>61</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="D42" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="60" customHeight="1">
-      <c r="A43" s="22">
-        <v>9</v>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="19">
+        <v>11</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D43" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="60" customHeight="1">
-      <c r="A44" s="22">
-        <v>9</v>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="19">
+        <v>11</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D44" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="60" customHeight="1">
-      <c r="A45" s="22">
-        <v>9</v>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="19">
+        <v>11</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D45" s="11">
         <v>-100</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="3" customHeight="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-    </row>
-    <row r="47" spans="1:4" ht="60" customHeight="1">
-      <c r="A47" s="21">
-        <v>10</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="12">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="18">
+        <v>12</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="60" customHeight="1">
-      <c r="A48" s="21">
-        <v>10</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" s="11">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="18">
+        <v>12</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="60" customHeight="1">
-      <c r="A49" s="21">
-        <v>10</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D49" s="12">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="18">
+        <v>12</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" s="12">
         <v>-50</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="48" customHeight="1">
-      <c r="A50" s="21">
-        <v>10</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="11">
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="20">
+        <v>12</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="13">
         <v>-100</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="3" customHeight="1">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-    </row>
-    <row r="52" spans="1:4" ht="60" customHeight="1">
-      <c r="A52" s="22">
-        <v>11</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D52" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="60" customHeight="1">
-      <c r="A53" s="22">
-        <v>11</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53" s="11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="60" customHeight="1">
-      <c r="A54" s="22">
-        <v>11</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="12">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="60" customHeight="1">
-      <c r="A55" s="22">
-        <v>11</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D55" s="11">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="3" customHeight="1">
-      <c r="A56" s="18"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-    </row>
-    <row r="57" spans="1:4" ht="60" customHeight="1">
-      <c r="A57" s="21">
-        <v>12</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="60" customHeight="1">
-      <c r="A58" s="21">
-        <v>12</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D58" s="11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="60" customHeight="1">
-      <c r="A59" s="21">
-        <v>12</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D59" s="12">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="60" customHeight="1">
-      <c r="A60" s="23">
-        <v>12</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D60" s="13">
-        <v>-100</v>
-      </c>
-    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>